<commit_message>
Divisão por 2 e correção de ruido inserido
</commit_message>
<xml_diff>
--- a/phase_noise_calc.xlsx
+++ b/phase_noise_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asavbrm-my.sharepoint.com/personal/andersonfw_edu_unisinos_br/Documents/UNISINOS/TCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{172DA3FB-88F8-4B0B-9156-93835AE2E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{172DA3FB-88F8-4B0B-9156-93835AE2E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA10474C-2712-436C-8389-D1791638AB4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9FD561C1-5AF9-477C-8B73-808FF998BF67}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>sensibilidade</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>LO phase noise @</t>
+  </si>
+  <si>
+    <t>LO phase noise @1M</t>
+  </si>
+  <si>
+    <t>LO phase noise @2M</t>
+  </si>
+  <si>
+    <t>LO phase noise @3M</t>
+  </si>
+  <si>
+    <t>C/I @1M</t>
+  </si>
+  <si>
+    <t>C/I @2M</t>
+  </si>
+  <si>
+    <t>C/I @3M</t>
+  </si>
+  <si>
+    <t>In band Noise</t>
   </si>
 </sst>
 </file>
@@ -101,10 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,6 +140,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8696</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>56545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C565410B-AC51-6D20-BB53-DF8F10D5F4A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="2838450"/>
+          <a:ext cx="6628571" cy="4838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>256392</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>109964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{891D6254-0486-BFCA-2C71-DED186A77D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6994071" y="2272393"/>
+          <a:ext cx="6284357" cy="2028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>35892</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>52810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6E2B42-4616-9E6A-8E5E-51192F6AA350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6898821" y="4463143"/>
+          <a:ext cx="6771428" cy="2066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EFE818-57D5-4E86-9F10-E4F4541C9F57}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +589,7 @@
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +602,14 @@
       <c r="G1">
         <v>-70</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,10 +620,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30000000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -473,8 +642,14 @@
       <c r="G3">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -488,7 +663,7 @@
         <v>-67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -499,10 +674,10 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -516,23 +691,23 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <f>10*LOG10(B6)</f>
         <v>53.010299956639813</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <f>10*LOG10(G6)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -544,11 +719,11 @@
         <v>4</v>
       </c>
       <c r="G8">
-        <f>-174 +G7+G5</f>
-        <v>-104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f>-174+G7</f>
+        <v>-114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -557,14 +732,14 @@
         <v>-99</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <f>G1+3</f>
-        <v>-67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f>-21-G7</f>
+        <v>-81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -573,14 +748,33 @@
         <v>-118.01029995663981</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <f>G10-(G4)-G7-G3</f>
-        <v>-77</v>
+        <f>-21-G7+I1</f>
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <f>-21-G7+I2</f>
+        <v>-98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <f>-21-G7+I3</f>
+        <v>-108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação de imagens do Loop Filter; Ajustes de simulação do ADPLL 5G;
</commit_message>
<xml_diff>
--- a/phase_noise_calc.xlsx
+++ b/phase_noise_calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asavbrm-my.sharepoint.com/personal/andersonfw_edu_unisinos_br/Documents/UNISINOS/TCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{172DA3FB-88F8-4B0B-9156-93835AE2E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA10474C-2712-436C-8389-D1791638AB4C}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{172DA3FB-88F8-4B0B-9156-93835AE2E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{703BF02B-B5A2-4F6F-97AF-781E0DAFF50F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9FD561C1-5AF9-477C-8B73-808FF998BF67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9FD561C1-5AF9-477C-8B73-808FF998BF67}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,20 +577,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EFE818-57D5-4E86-9F10-E4F4541C9F57}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,8 +609,11 @@
       <c r="I1">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -628,8 +632,11 @@
       <c r="I2">
         <v>-17</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -648,8 +655,11 @@
       <c r="I3">
         <v>-27</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -663,7 +673,7 @@
         <v>-67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -677,7 +687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -691,7 +701,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -702,12 +712,12 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f>10*LOG10(G6)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -723,7 +733,7 @@
         <v>-114</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -739,7 +749,7 @@
         <v>-81</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -755,7 +765,7 @@
         <v>-66</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>11</v>
       </c>
@@ -764,7 +774,7 @@
         <v>-98</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>12</v>
       </c>

</xml_diff>